<commit_message>
Able to replace all texts from dictionary
</commit_message>
<xml_diff>
--- a/automate/excel-to-doc/input.xlsx
+++ b/automate/excel-to-doc/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tanwaarpornthip/psuPortal/automate/excel-to-doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C41AC9CB-4D01-284D-A889-CA98EE292E2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0D1462-6AC2-FE42-AE12-774C042ABF6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1860" windowWidth="28040" windowHeight="17440" xr2:uid="{B384F9D7-1B30-B047-B10D-8C9199A999C2}"/>
+    <workbookView xWindow="5040" yWindow="2140" windowWidth="14140" windowHeight="17180" xr2:uid="{B384F9D7-1B30-B047-B10D-8C9199A999C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,28 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>Index</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Items</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Cost</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Stationery</t>
   </si>
@@ -64,6 +43,45 @@
   </si>
   <si>
     <t>Carrots</t>
+  </si>
+  <si>
+    <t>counts</t>
+  </si>
+  <si>
+    <t>bulbs</t>
+  </si>
+  <si>
+    <t>INDEX</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>ORGANIZATION</t>
+  </si>
+  <si>
+    <t>QUANTITY</t>
+  </si>
+  <si>
+    <t>UNIT</t>
+  </si>
+  <si>
+    <t>PRICE</t>
+  </si>
+  <si>
+    <t>COST</t>
+  </si>
+  <si>
+    <t>ITEM</t>
+  </si>
+  <si>
+    <t>COST_TEXT</t>
+  </si>
+  <si>
+    <t>ยี่สิบห้าบาท</t>
+  </si>
+  <si>
+    <t>สองบาท</t>
   </si>
 </sst>
 </file>
@@ -425,38 +443,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1189DC3C-6D58-7D42-AFC1-52BCFE0E394B}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -464,23 +491,29 @@
         <v>43470</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <v>5</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2">
         <v>5</v>
       </c>
-      <c r="G2">
-        <f>PRODUCT(E2:F2)</f>
+      <c r="H2">
+        <f>PRODUCT(E2:G2)</f>
         <v>25</v>
       </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -488,20 +521,26 @@
         <v>43753</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E3">
         <v>10</v>
       </c>
-      <c r="F3">
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3">
         <v>0.2</v>
       </c>
-      <c r="G3">
-        <f>PRODUCT(E3:F3)</f>
+      <c r="H3">
+        <f>PRODUCT(E3:G3)</f>
         <v>2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>